<commit_message>
marketing in a digital world
</commit_message>
<xml_diff>
--- a/MOOClist.xlsx
+++ b/MOOClist.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="240">
   <si>
     <t>#</t>
   </si>
@@ -724,6 +724,30 @@
   </si>
   <si>
     <t>Effective problem-solving and decision-making</t>
+  </si>
+  <si>
+    <t>Women in leadership: inspiring positive change</t>
+  </si>
+  <si>
+    <t>Content strategy for professionals 1: engaging audiences for your organization</t>
+  </si>
+  <si>
+    <t>Northwestern University</t>
+  </si>
+  <si>
+    <t>Content strategy for professionals</t>
+  </si>
+  <si>
+    <t>Introduction to project management principles and practices</t>
+  </si>
+  <si>
+    <t>Initiation and planning projects</t>
+  </si>
+  <si>
+    <t>Budgeting and scheduling projects</t>
+  </si>
+  <si>
+    <t>Managing risks and changes</t>
   </si>
 </sst>
 </file>
@@ -890,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1142,9 +1166,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1182,20 +1203,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1208,6 +1220,24 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1521,7 +1551,7 @@
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="9" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="96" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="95" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="17"/>
     <col min="12" max="12" width="17.140625" style="17" customWidth="1"/>
@@ -1990,7 +2020,7 @@
       <c r="G13" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="H13" s="101">
+      <c r="H13" s="100">
         <v>1</v>
       </c>
       <c r="I13" s="12" t="s">
@@ -3146,7 +3176,7 @@
       <c r="N42" s="8"/>
     </row>
     <row r="43" spans="1:14" ht="26.25" customHeight="1">
-      <c r="A43" s="95"/>
+      <c r="A43" s="94"/>
       <c r="B43" s="14">
         <f>B42+1</f>
         <v>41</v>
@@ -3187,7 +3217,7 @@
       <c r="N43" s="8"/>
     </row>
     <row r="44" spans="1:14" ht="26.25" customHeight="1">
-      <c r="A44" s="95"/>
+      <c r="A44" s="94"/>
       <c r="B44" s="14">
         <f>B43+1</f>
         <v>42</v>
@@ -3210,7 +3240,7 @@
       <c r="H44" s="40">
         <v>0.83</v>
       </c>
-      <c r="I44" s="97" t="s">
+      <c r="I44" s="96" t="s">
         <v>86</v>
       </c>
       <c r="J44" s="25" t="s">
@@ -3312,221 +3342,221 @@
         <f>B46+1</f>
         <v>45</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="36">
-        <v>9</v>
-      </c>
-      <c r="F47" s="24">
-        <v>10</v>
+      <c r="C47" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="E47" s="35">
+        <v>6</v>
+      </c>
+      <c r="F47" s="52">
+        <v>4</v>
       </c>
       <c r="G47" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H47" s="40">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J47" s="30" t="s">
-        <v>80</v>
+        <v>0.1</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>82</v>
       </c>
       <c r="K47" s="47">
         <f>E47*F47</f>
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="L47" s="48">
         <f>ROUND(K47/28,1)</f>
-        <v>3.2</v>
+        <v>0.9</v>
       </c>
       <c r="M47" s="7"/>
       <c r="N47" s="8"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" ht="25.5">
       <c r="B48" s="14">
         <f>B47+1</f>
         <v>46</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="36">
+        <v>9</v>
+      </c>
+      <c r="F48" s="24">
         <v>10</v>
       </c>
-      <c r="E48" s="36">
-        <v>10</v>
-      </c>
-      <c r="F48" s="24">
-        <v>3</v>
-      </c>
-      <c r="G48" s="43" t="s">
-        <v>86</v>
+      <c r="G48" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="H48" s="40">
-        <v>0.82699999999999996</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K48" s="47">
         <f>E48*F48</f>
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="L48" s="48">
         <f>ROUND(K48/28,1)</f>
-        <v>1.1000000000000001</v>
+        <v>3.2</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="8"/>
     </row>
-    <row r="49" spans="1:14" ht="25.5">
+    <row r="49" spans="1:14">
       <c r="B49" s="14">
         <f>B48+1</f>
         <v>47</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="12" t="s">
+      <c r="C49" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="35">
-        <v>8</v>
-      </c>
-      <c r="F49" s="52">
-        <v>6</v>
-      </c>
-      <c r="G49" s="42" t="s">
+      <c r="E49" s="36">
+        <v>10</v>
+      </c>
+      <c r="F49" s="24">
+        <v>3</v>
+      </c>
+      <c r="G49" s="43" t="s">
         <v>86</v>
       </c>
       <c r="H49" s="40">
-        <v>0.88400000000000001</v>
-      </c>
-      <c r="I49" s="12" t="s">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="I49" s="13" t="s">
         <v>86</v>
       </c>
       <c r="J49" s="30" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="K49" s="47">
         <f>E49*F49</f>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="L49" s="48">
         <f>ROUND(K49/28,1)</f>
-        <v>1.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M49" s="7"/>
       <c r="N49" s="8"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" ht="25.5">
       <c r="B50" s="14">
         <f>B49+1</f>
         <v>48</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" s="36">
-        <v>5</v>
-      </c>
-      <c r="F50" s="24">
-        <v>3</v>
-      </c>
-      <c r="G50" s="43" t="s">
+      <c r="C50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="35">
+        <v>8</v>
+      </c>
+      <c r="F50" s="52">
+        <v>6</v>
+      </c>
+      <c r="G50" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="H50" s="41">
-        <v>0.87</v>
+      <c r="H50" s="40">
+        <v>0.88400000000000001</v>
       </c>
       <c r="I50" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J50" s="25" t="s">
-        <v>84</v>
+      <c r="J50" s="30" t="s">
+        <v>64</v>
       </c>
       <c r="K50" s="47">
         <f>E50*F50</f>
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="L50" s="48">
         <f>ROUND(K50/28,1)</f>
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:14" ht="25.5">
+    <row r="51" spans="1:14">
       <c r="B51" s="14">
         <f>B50+1</f>
         <v>49</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" s="12" t="s">
+      <c r="C51" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="35">
+      <c r="E51" s="36">
         <v>5</v>
       </c>
-      <c r="F51" s="52">
-        <v>9</v>
-      </c>
-      <c r="G51" s="42" t="s">
+      <c r="F51" s="24">
+        <v>3</v>
+      </c>
+      <c r="G51" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="H51" s="40">
-        <v>0.78</v>
+      <c r="H51" s="41">
+        <v>0.87</v>
       </c>
       <c r="I51" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J51" s="30" t="s">
+      <c r="J51" s="25" t="s">
         <v>84</v>
       </c>
       <c r="K51" s="47">
         <f>E51*F51</f>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="L51" s="48">
         <f>ROUND(K51/28,1)</f>
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" ht="25.5">
       <c r="B52" s="14">
         <f>B51+1</f>
         <v>50</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="55" t="s">
+      <c r="C52" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="52">
         <v>5</v>
       </c>
-      <c r="F52" s="24">
+      <c r="F52" s="52">
         <v>9</v>
       </c>
       <c r="G52" s="42" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="H52" s="53">
-        <v>0.89300000000000002</v>
+        <v>0.78</v>
       </c>
       <c r="I52" s="56" t="s">
         <v>86</v>
@@ -3543,42 +3573,42 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="25.5">
+    <row r="53" spans="1:14">
       <c r="B53" s="14">
         <f>B52+1</f>
         <v>51</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="D53" s="55" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="E53" s="24">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F53" s="24">
-        <v>6</v>
-      </c>
-      <c r="G53" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H53" s="53">
-        <v>0.95299999999999996</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="I53" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J53" s="65" t="s">
-        <v>191</v>
+      <c r="J53" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="K53" s="47">
         <f>E53*F53</f>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L53" s="48">
         <f>ROUND(K53/28,1)</f>
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="25.5">
@@ -3588,36 +3618,36 @@
         <v>52</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>214</v>
+        <v>106</v>
+      </c>
+      <c r="D54" s="55" t="s">
+        <v>154</v>
       </c>
       <c r="E54" s="24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F54" s="24">
         <v>6</v>
       </c>
-      <c r="G54" s="42" t="s">
-        <v>228</v>
+      <c r="G54" s="43" t="s">
+        <v>112</v>
       </c>
       <c r="H54" s="53">
-        <v>0.95</v>
-      </c>
-      <c r="I54" s="55" t="s">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="I54" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J54" s="23" t="s">
-        <v>82</v>
+      <c r="J54" s="65" t="s">
+        <v>191</v>
       </c>
       <c r="K54" s="47">
         <f>E54*F54</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="L54" s="48">
         <f>ROUND(K54/28,1)</f>
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="25.5">
@@ -3627,153 +3657,153 @@
         <v>53</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D55" s="55" t="s">
-        <v>7</v>
+        <v>213</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>214</v>
       </c>
       <c r="E55" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F55" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G55" s="42" t="s">
         <v>228</v>
       </c>
       <c r="H55" s="53">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="I55" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="J55" s="65" t="s">
-        <v>79</v>
+        <v>86</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="K55" s="47">
         <f>E55*F55</f>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L55" s="48">
         <f>ROUND(K55/28,1)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="26.25">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="25.5">
       <c r="A56" s="7"/>
       <c r="B56" s="14">
         <f>B55+1</f>
         <v>54</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" s="65" t="s">
+      <c r="C56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="E56" s="52">
-        <v>1</v>
-      </c>
-      <c r="F56" s="52">
-        <v>8</v>
+      <c r="E56" s="24">
+        <v>5</v>
+      </c>
+      <c r="F56" s="24">
+        <v>4</v>
       </c>
       <c r="G56" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H56" s="53">
         <v>1</v>
       </c>
-      <c r="I56" s="56" t="s">
-        <v>217</v>
+      <c r="I56" s="55" t="s">
+        <v>65</v>
       </c>
       <c r="J56" s="65" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K56" s="47">
         <f>E56*F56</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L56" s="48">
         <f>ROUND(K56/28,1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="26.25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="38.25">
       <c r="A57" s="7"/>
       <c r="B57" s="14">
         <f>B56+1</f>
         <v>55</v>
       </c>
-      <c r="C57" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="D57" s="25" t="s">
+      <c r="C57" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F57" s="52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G57" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H57" s="40">
+      <c r="H57" s="98">
         <v>1</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="J57" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K57" s="47">
         <f>E57*F57</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L57" s="48">
         <f>ROUND(K57/28,1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="25.5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="26.25">
       <c r="A58" s="7"/>
       <c r="B58" s="14">
         <f>B57+1</f>
         <v>56</v>
       </c>
-      <c r="C58" s="25" t="s">
-        <v>104</v>
+      <c r="C58" s="54" t="s">
+        <v>225</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="36">
-        <v>5</v>
-      </c>
-      <c r="F58" s="24">
-        <v>4</v>
+      <c r="E58" s="35">
+        <v>1</v>
+      </c>
+      <c r="F58" s="52">
+        <v>8</v>
       </c>
       <c r="G58" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H58" s="40">
-        <v>0.99</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>217</v>
       </c>
       <c r="J58" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K58" s="47">
         <f>E58*F58</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L58" s="48">
         <f>ROUND(K58/28,1)</f>
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="26.25">
@@ -3783,7 +3813,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D59" s="65" t="s">
         <v>7</v>
@@ -3815,82 +3845,82 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" ht="25.5">
       <c r="A60" s="7"/>
       <c r="B60" s="14">
         <f>B59+1</f>
         <v>58</v>
       </c>
-      <c r="C60" s="54" t="s">
-        <v>224</v>
+      <c r="C60" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="35">
-        <v>1</v>
-      </c>
-      <c r="F60" s="52">
-        <v>8</v>
+      <c r="E60" s="36">
+        <v>5</v>
+      </c>
+      <c r="F60" s="24">
+        <v>4</v>
       </c>
       <c r="G60" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H60" s="40">
-        <v>1</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>217</v>
+        <v>0.99</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="J60" s="25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K60" s="47">
         <f>E60*F60</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L60" s="48">
         <f>ROUND(K60/28,1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="25.5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="26.25">
       <c r="A61" s="7"/>
       <c r="B61" s="14">
         <f>B60+1</f>
         <v>59</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="12" t="s">
+      <c r="C61" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="36">
-        <v>5</v>
-      </c>
-      <c r="F61" s="24">
-        <v>4</v>
+      <c r="E61" s="35">
+        <v>1</v>
+      </c>
+      <c r="F61" s="52">
+        <v>8</v>
       </c>
       <c r="G61" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H61" s="40">
-        <v>0.93</v>
-      </c>
-      <c r="I61" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J61" s="30" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="J61" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="K61" s="47">
         <f>E61*F61</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L61" s="48">
         <f>ROUND(K61/28,1)</f>
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3900,7 +3930,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="54" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>7</v>
@@ -3932,199 +3962,199 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" ht="25.5">
       <c r="A63" s="7"/>
       <c r="B63" s="14">
         <f>B62+1</f>
         <v>61</v>
       </c>
-      <c r="C63" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="D63" s="25" t="s">
+      <c r="C63" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="42">
-        <v>1</v>
-      </c>
-      <c r="F63" s="52">
-        <v>8</v>
+      <c r="E63" s="43">
+        <v>5</v>
+      </c>
+      <c r="F63" s="24">
+        <v>4</v>
       </c>
       <c r="G63" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H63" s="40">
-        <v>1</v>
-      </c>
-      <c r="I63" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="J63" s="25" t="s">
-        <v>85</v>
+        <v>0.93</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J63" s="30" t="s">
+        <v>79</v>
       </c>
       <c r="K63" s="47">
         <f>E63*F63</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L63" s="48">
         <f>ROUND(K63/28,1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="25.5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="7"/>
       <c r="B64" s="14">
         <f>B63+1</f>
         <v>62</v>
       </c>
-      <c r="C64" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D64" s="13" t="s">
+      <c r="C64" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="36">
-        <v>5</v>
-      </c>
-      <c r="F64" s="24">
-        <v>7</v>
+      <c r="E64" s="35">
+        <v>1</v>
+      </c>
+      <c r="F64" s="52">
+        <v>8</v>
       </c>
       <c r="G64" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H64" s="101">
-        <v>0.97</v>
-      </c>
-      <c r="I64" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="J64" s="12" t="s">
-        <v>82</v>
+        <v>112</v>
+      </c>
+      <c r="H64" s="40">
+        <v>1</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="J64" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="K64" s="47">
         <f>E64*F64</f>
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="L64" s="48">
         <f>ROUND(K64/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="25.5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="7"/>
       <c r="B65" s="14">
         <f>B64+1</f>
         <v>63</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D65" s="13" t="s">
+      <c r="C65" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="D65" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="36">
-        <v>5</v>
-      </c>
-      <c r="F65" s="24">
-        <v>4</v>
+      <c r="E65" s="35">
+        <v>1</v>
+      </c>
+      <c r="F65" s="52">
+        <v>8</v>
       </c>
       <c r="G65" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H65" s="40">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="I65" s="13" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>217</v>
       </c>
       <c r="J65" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K65" s="47">
         <f>E65*F65</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L65" s="48">
         <f>ROUND(K65/28,1)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="25.5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="38.25">
       <c r="A66" s="7"/>
       <c r="B66" s="35">
         <f>B65+1</f>
         <v>64</v>
       </c>
-      <c r="C66" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="D66" s="25" t="s">
+      <c r="C66" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F66" s="52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G66" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H66" s="40">
+      <c r="H66" s="98">
         <v>1</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="J66" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K66" s="47">
         <f>E66*F66</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L66" s="48">
         <f>ROUND(K66/28,1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="38.25">
       <c r="A67" s="7"/>
       <c r="B67" s="35">
         <f>B66+1</f>
         <v>65</v>
       </c>
-      <c r="C67" s="54" t="s">
-        <v>230</v>
-      </c>
-      <c r="D67" s="25" t="s">
+      <c r="C67" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E67" s="35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F67" s="52">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G67" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H67" s="40">
+      <c r="H67" s="98">
         <v>1</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="J67" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K67" s="47">
         <f>E67*F67</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L67" s="48">
         <f>ROUND(K67/28,1)</f>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="25.5">
@@ -4133,37 +4163,37 @@
         <f>B67+1</f>
         <v>66</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="12" t="s">
+      <c r="C68" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="35">
-        <v>11</v>
-      </c>
-      <c r="F68" s="52">
-        <v>4</v>
+      <c r="E68" s="36">
+        <v>5</v>
+      </c>
+      <c r="F68" s="24">
+        <v>7</v>
       </c>
       <c r="G68" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="H68" s="100">
+        <v>0.97</v>
+      </c>
+      <c r="I68" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="H68" s="40">
-        <v>0.751</v>
-      </c>
-      <c r="I68" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J68" s="30" t="s">
-        <v>83</v>
+      <c r="J68" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="K68" s="47">
         <f>E68*F68</f>
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="L68" s="48">
         <f>ROUND(K68/28,1)</f>
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="25.5">
@@ -4172,37 +4202,37 @@
         <f>B68+1</f>
         <v>67</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="12" t="s">
+      <c r="C69" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="35">
-        <v>11</v>
-      </c>
-      <c r="F69" s="52">
+      <c r="E69" s="36">
+        <v>5</v>
+      </c>
+      <c r="F69" s="24">
         <v>4</v>
       </c>
       <c r="G69" s="42" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="H69" s="40">
-        <v>0.746</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J69" s="30" t="s">
-        <v>83</v>
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J69" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="K69" s="47">
         <f>E69*F69</f>
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="L69" s="48">
         <f>ROUND(K69/28,1)</f>
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="25.5">
@@ -4211,44 +4241,47 @@
         <f>B69+1</f>
         <v>68</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="12" t="s">
+      <c r="C70" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D70" s="25" t="s">
         <v>7</v>
       </c>
       <c r="E70" s="42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F70" s="52">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G70" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H70" s="40">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="J70" s="25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K70" s="47">
         <f>E70*F70</f>
-        <v>15</v>
-      </c>
-      <c r="L70" s="28"/>
-    </row>
-    <row r="71" spans="1:12" ht="39">
+        <v>8</v>
+      </c>
+      <c r="L70" s="48">
+        <f>ROUND(K70/28,1)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="7"/>
       <c r="B71" s="35">
         <f>B70+1</f>
         <v>69</v>
       </c>
       <c r="C71" s="54" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>7</v>
@@ -4280,43 +4313,43 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" ht="25.5">
       <c r="A72" s="7"/>
       <c r="B72" s="35">
         <f>B71+1</f>
         <v>70</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E72" s="35">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F72" s="52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G72" s="42" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="H72" s="40">
-        <v>0.82599999999999996</v>
+        <v>0.751</v>
       </c>
       <c r="I72" s="12" t="s">
         <v>86</v>
       </c>
       <c r="J72" s="30" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="K72" s="47">
         <f>E72*F72</f>
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="L72" s="48">
         <f>ROUND(K72/28,1)</f>
-        <v>0.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="25.5">
@@ -4325,37 +4358,37 @@
         <f>B72+1</f>
         <v>71</v>
       </c>
-      <c r="C73" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="D73" s="65" t="s">
-        <v>141</v>
+      <c r="C73" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="56" t="s">
+        <v>7</v>
       </c>
       <c r="E73" s="52">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F73" s="52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G73" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H73" s="107">
-        <v>0.93</v>
-      </c>
-      <c r="I73" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="J73" s="65" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="H73" s="53">
+        <v>0.746</v>
+      </c>
+      <c r="I73" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J73" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="K73" s="47">
         <f>E73*F73</f>
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="L73" s="49">
         <f>ROUND(K73/28,1)</f>
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="25.5">
@@ -4365,153 +4398,150 @@
         <v>72</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E74" s="35">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F74" s="52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G74" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H74" s="40">
-        <v>0.93700000000000006</v>
+        <v>0.96</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J74" s="30" t="s">
-        <v>83</v>
+        <v>163</v>
+      </c>
+      <c r="J74" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="K74" s="47">
         <f>E74*F74</f>
-        <v>48</v>
-      </c>
-      <c r="L74" s="48">
-        <f>ROUND(K74/28,1)</f>
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="25.5">
+        <v>15</v>
+      </c>
+      <c r="L74" s="28"/>
+    </row>
+    <row r="75" spans="1:12" ht="39">
       <c r="A75" s="7"/>
       <c r="B75" s="14">
         <f>B74+1</f>
         <v>73</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D75" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="24">
-        <v>4</v>
-      </c>
-      <c r="F75" s="24">
-        <v>6</v>
-      </c>
-      <c r="G75" s="43" t="s">
-        <v>86</v>
+      <c r="C75" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="52">
+        <v>1</v>
+      </c>
+      <c r="F75" s="52">
+        <v>8</v>
+      </c>
+      <c r="G75" s="42" t="s">
+        <v>112</v>
       </c>
       <c r="H75" s="53">
-        <v>0.91</v>
-      </c>
-      <c r="I75" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="J75" s="23" t="s">
-        <v>64</v>
+        <v>1</v>
+      </c>
+      <c r="I75" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="J75" s="65" t="s">
+        <v>85</v>
       </c>
       <c r="K75" s="47">
         <f>E75*F75</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="L75" s="48">
         <f>ROUND(K75/28,1)</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="25.5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="7"/>
       <c r="B76" s="14">
         <f>B75+1</f>
         <v>74</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D76" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="24">
-        <v>8</v>
-      </c>
-      <c r="F76" s="24">
-        <v>6</v>
+      <c r="C76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="52">
+        <v>5</v>
+      </c>
+      <c r="F76" s="52">
+        <v>2</v>
       </c>
       <c r="G76" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H76" s="53">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="I76" s="55" t="s">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="I76" s="56" t="s">
         <v>86</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="K76" s="47">
         <f>E76*F76</f>
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="L76" s="48">
         <f>ROUND(K76/28,1)</f>
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="25.5">
       <c r="A77" s="7"/>
       <c r="B77" s="14">
         <f>B76+1</f>
         <v>75</v>
       </c>
-      <c r="C77" s="20" t="s">
-        <v>117</v>
+      <c r="C77" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="E77" s="42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F77" s="52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G77" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="H77" s="40">
-        <v>1</v>
-      </c>
-      <c r="I77" s="12" t="s">
-        <v>86</v>
+      <c r="H77" s="110">
+        <v>0.93</v>
+      </c>
+      <c r="I77" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K77" s="47">
         <f>E77*F77</f>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="L77" s="48">
         <f>ROUND(K77/28,1)</f>
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="25.5">
@@ -4521,36 +4551,36 @@
         <v>76</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="D78" s="56" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="E78" s="52">
+        <v>8</v>
+      </c>
+      <c r="F78" s="52">
         <v>6</v>
       </c>
-      <c r="F78" s="52">
-        <v>2</v>
-      </c>
-      <c r="G78" s="104" t="s">
-        <v>40</v>
+      <c r="G78" s="42" t="s">
+        <v>112</v>
       </c>
       <c r="H78" s="53">
-        <v>0.74</v>
-      </c>
-      <c r="I78" s="39" t="s">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="I78" s="12" t="s">
         <v>86</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K78" s="47">
         <f>E78*F78</f>
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="L78" s="48">
         <f>ROUND(K78/28,1)</f>
-        <v>0.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="25.5">
@@ -4560,36 +4590,36 @@
         <v>77</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>76</v>
+        <v>193</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="E79" s="36">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F79" s="24">
         <v>6</v>
       </c>
-      <c r="G79" s="42" t="s">
-        <v>112</v>
+      <c r="G79" s="43" t="s">
+        <v>86</v>
       </c>
       <c r="H79" s="40">
-        <v>0.83299999999999996</v>
+        <v>0.91</v>
       </c>
       <c r="I79" s="13" t="s">
-        <v>86</v>
+        <v>195</v>
       </c>
       <c r="J79" s="30" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="K79" s="47">
         <f>E79*F79</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="L79" s="48">
         <f>ROUND(K79/28,1)</f>
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="25.5">
@@ -4598,25 +4628,25 @@
         <f>B79+1</f>
         <v>78</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D80" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="E80" s="52">
-        <v>5</v>
-      </c>
-      <c r="F80" s="52">
-        <v>4</v>
+      <c r="C80" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D80" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="24">
+        <v>8</v>
+      </c>
+      <c r="F80" s="24">
+        <v>6</v>
       </c>
       <c r="G80" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H80" s="53">
-        <v>0.9</v>
-      </c>
-      <c r="I80" s="56" t="s">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I80" s="55" t="s">
         <v>86</v>
       </c>
       <c r="J80" s="23" t="s">
@@ -4624,30 +4654,30 @@
       </c>
       <c r="K80" s="47">
         <f>E80*F80</f>
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="L80" s="48">
         <f>ROUND(K80/28,1)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="38.25">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="7"/>
       <c r="B81" s="14">
         <f>B80+1</f>
         <v>79</v>
       </c>
-      <c r="C81" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="D81" s="56" t="s">
-        <v>27</v>
+      <c r="C81" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D81" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="E81" s="52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="52">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G81" s="42" t="s">
         <v>228</v>
@@ -4656,447 +4686,447 @@
         <v>1</v>
       </c>
       <c r="I81" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="J81" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="J81" s="65" t="s">
         <v>82</v>
       </c>
       <c r="K81" s="47">
         <f>E81*F81</f>
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="L81" s="48">
         <f>ROUND(K81/28,1)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="38.25">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="25.5">
       <c r="A82" s="7"/>
       <c r="B82" s="14">
         <f>B81+1</f>
         <v>80</v>
       </c>
-      <c r="C82" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D82" s="65" t="s">
-        <v>27</v>
+      <c r="C82" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D82" s="56" t="s">
+        <v>76</v>
       </c>
       <c r="E82" s="52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F82" s="52">
-        <v>5</v>
-      </c>
-      <c r="G82" s="42" t="s">
-        <v>228</v>
+        <v>2</v>
+      </c>
+      <c r="G82" s="102" t="s">
+        <v>40</v>
       </c>
       <c r="H82" s="53">
-        <v>0.95</v>
-      </c>
-      <c r="I82" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="J82" s="65" t="s">
-        <v>82</v>
+        <v>0.74</v>
+      </c>
+      <c r="I82" s="113" t="s">
+        <v>86</v>
+      </c>
+      <c r="J82" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="K82" s="47">
         <f>E82*F82</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="L82" s="48">
         <f>ROUND(K82/28,1)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="38.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="25.5">
       <c r="A83" s="7"/>
       <c r="B83" s="14">
         <f>B82+1</f>
         <v>81</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D83" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="E83" s="52">
-        <v>4</v>
-      </c>
-      <c r="F83" s="52">
-        <v>5</v>
+      <c r="C83" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E83" s="24">
+        <v>6</v>
+      </c>
+      <c r="F83" s="24">
+        <v>6</v>
       </c>
       <c r="G83" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H83" s="53">
-        <v>0.98</v>
-      </c>
-      <c r="I83" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="J83" s="65" t="s">
-        <v>82</v>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="I83" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="J83" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="K83" s="47">
         <f>E83*F83</f>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L83" s="48">
         <f>ROUND(K83/28,1)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="25.5">
       <c r="A84" s="7"/>
       <c r="B84" s="14">
         <f>B83+1</f>
         <v>82</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>34</v>
+        <v>187</v>
       </c>
       <c r="D84" s="56" t="s">
-        <v>35</v>
+        <v>188</v>
       </c>
       <c r="E84" s="52">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F84" s="52">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G84" s="42" t="s">
         <v>228</v>
       </c>
       <c r="H84" s="53">
-        <v>0.90800000000000003</v>
+        <v>0.9</v>
       </c>
       <c r="I84" s="56" t="s">
         <v>86</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="K84" s="47">
         <f>E84*F84</f>
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="L84" s="48">
         <f>ROUND(K84/28,1)</f>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="25.5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="38.25">
       <c r="A85" s="7"/>
       <c r="B85" s="14">
         <f>B84+1</f>
         <v>83</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D85" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="E85" s="24">
+      <c r="C85" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="52">
         <v>6</v>
       </c>
-      <c r="F85" s="24">
-        <v>4</v>
-      </c>
-      <c r="G85" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="H85" s="82">
-        <v>0.92</v>
+      <c r="F85" s="52">
+        <v>7</v>
+      </c>
+      <c r="G85" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="H85" s="53">
+        <v>1</v>
       </c>
       <c r="I85" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="J85" s="65" t="s">
-        <v>210</v>
+        <v>122</v>
+      </c>
+      <c r="J85" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="K85" s="47">
         <f>E85*F85</f>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L85" s="48">
         <f>ROUND(K85/28,1)</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="26.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="38.25">
       <c r="A86" s="7"/>
       <c r="B86" s="14">
         <f>B85+1</f>
         <v>84</v>
       </c>
-      <c r="C86" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="D86" s="65" t="s">
-        <v>119</v>
+      <c r="C86" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D86" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="E86" s="52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F86" s="52">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G86" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H86" s="53">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="I86" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="J86" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="J86" s="23" t="s">
         <v>82</v>
       </c>
       <c r="K86" s="47">
         <f>E86*F86</f>
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="L86" s="48">
         <f>ROUND(K86/28,1)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="38.25">
       <c r="A87" s="7"/>
       <c r="B87" s="14">
         <f>B86+1</f>
         <v>85</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D87" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="E87" s="24">
-        <v>6</v>
-      </c>
-      <c r="F87" s="24">
-        <v>6</v>
-      </c>
-      <c r="G87" s="43" t="s">
-        <v>112</v>
+      <c r="C87" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D87" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="52">
+        <v>4</v>
+      </c>
+      <c r="F87" s="52">
+        <v>5</v>
+      </c>
+      <c r="G87" s="42" t="s">
+        <v>228</v>
       </c>
       <c r="H87" s="53">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="I87" s="56" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="J87" s="65" t="s">
         <v>82</v>
       </c>
       <c r="K87" s="47">
         <f>E87*F87</f>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L87" s="48">
         <f>ROUND(K87/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="38.25">
       <c r="A88" s="7"/>
       <c r="B88" s="14">
         <f>B87+1</f>
         <v>86</v>
       </c>
-      <c r="C88" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D88" s="55" t="s">
-        <v>130</v>
+      <c r="C88" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88" s="65" t="s">
+        <v>27</v>
       </c>
       <c r="E88" s="52">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F88" s="52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G88" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H88" s="53">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="I88" s="56" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="J88" s="65" t="s">
         <v>82</v>
       </c>
       <c r="K88" s="47">
         <f>E88*F88</f>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L88" s="48">
         <f>ROUND(K88/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="25.5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="7"/>
       <c r="B89" s="14">
         <f>B88+1</f>
         <v>87</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>165</v>
+        <v>34</v>
       </c>
       <c r="D89" s="56" t="s">
-        <v>166</v>
+        <v>35</v>
       </c>
       <c r="E89" s="52">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F89" s="52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G89" s="42" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="H89" s="53">
-        <v>1</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="I89" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J89" s="65" t="s">
-        <v>81</v>
+      <c r="J89" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="K89" s="47">
         <f>E89*F89</f>
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="L89" s="48">
         <f>ROUND(K89/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="25.5">
       <c r="A90" s="7"/>
       <c r="B90" s="14">
         <f>B89+1</f>
         <v>88</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="D90" s="55" t="s">
-        <v>146</v>
-      </c>
-      <c r="E90" s="52">
+        <v>35</v>
+      </c>
+      <c r="E90" s="24">
         <v>6</v>
       </c>
-      <c r="F90" s="52">
-        <v>6</v>
-      </c>
-      <c r="G90" s="42" t="s">
+      <c r="F90" s="24">
+        <v>4</v>
+      </c>
+      <c r="G90" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="H90" s="53">
-        <v>0.89</v>
+      <c r="H90" s="82">
+        <v>0.92</v>
       </c>
       <c r="I90" s="56" t="s">
         <v>86</v>
       </c>
       <c r="J90" s="65" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="K90" s="47">
         <f>E90*F90</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="L90" s="48">
         <f>ROUND(K90/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="26.25">
       <c r="A91" s="7"/>
       <c r="B91" s="14">
         <f>B90+1</f>
         <v>89</v>
       </c>
-      <c r="C91" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91" s="36">
-        <v>9</v>
-      </c>
-      <c r="F91" s="24">
-        <v>6</v>
+      <c r="C91" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E91" s="35">
+        <v>5</v>
+      </c>
+      <c r="F91" s="52">
+        <v>3</v>
       </c>
       <c r="G91" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H91" s="53">
-        <v>1</v>
-      </c>
-      <c r="I91" s="55" t="s">
+        <v>0.91</v>
+      </c>
+      <c r="I91" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J91" s="23" t="s">
+      <c r="J91" s="65" t="s">
         <v>82</v>
       </c>
       <c r="K91" s="48">
         <f>E91*F91</f>
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="L91" s="48">
         <f>ROUND(K91/28,1)</f>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="25.5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="7"/>
       <c r="B92" s="14">
         <f>B91+1</f>
         <v>90</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="D92" s="55" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="E92" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" s="24">
-        <v>4</v>
-      </c>
-      <c r="G92" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G92" s="43" t="s">
         <v>112</v>
       </c>
       <c r="H92" s="53">
-        <v>0.97499999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="I92" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J92" s="23" t="s">
+      <c r="J92" s="65" t="s">
         <v>82</v>
       </c>
       <c r="K92" s="47">
         <f>E92*F92</f>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="L92" s="48">
         <f>ROUND(K92/28,1)</f>
-        <v>1</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -5105,101 +5135,101 @@
         <f>B92+1</f>
         <v>91</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>124</v>
+      <c r="C93" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="D93" s="55" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="E93" s="52">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F93" s="52">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G93" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H93" s="53">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="I93" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J93" s="30" t="s">
+      <c r="J93" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K93" s="47">
         <f>E93*F93</f>
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="L93" s="48">
         <f>ROUND(K93/28,1)</f>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="25.5">
       <c r="A94" s="7"/>
       <c r="B94" s="14">
         <f>B93+1</f>
         <v>92</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="E94" s="35">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F94" s="52">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G94" s="42" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="H94" s="53">
-        <v>0.90500000000000003</v>
+        <v>1</v>
       </c>
       <c r="I94" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J94" s="23" t="s">
-        <v>82</v>
+      <c r="J94" s="65" t="s">
+        <v>81</v>
       </c>
       <c r="K94" s="48">
         <f>E94*F94</f>
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="L94" s="48">
         <f>ROUND(K94/28,1)</f>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="25.5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="7"/>
       <c r="B95" s="14">
         <f>B94+1</f>
         <v>93</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E95" s="24">
-        <v>4</v>
-      </c>
-      <c r="F95" s="24">
-        <v>3</v>
+        <v>146</v>
+      </c>
+      <c r="E95" s="52">
+        <v>6</v>
+      </c>
+      <c r="F95" s="52">
+        <v>6</v>
       </c>
       <c r="G95" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H95" s="53">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="I95" s="56" t="s">
         <v>86</v>
@@ -5209,50 +5239,50 @@
       </c>
       <c r="K95" s="48">
         <f>E95*F95</f>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="L95" s="48">
         <f>ROUND(K95/28,1)</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" ht="26.25">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="7"/>
       <c r="B96" s="14">
         <f>B95+1</f>
         <v>94</v>
       </c>
-      <c r="C96" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D96" s="105" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="52">
-        <v>4</v>
-      </c>
-      <c r="F96" s="52">
-        <v>4</v>
+      <c r="C96" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D96" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="E96" s="24">
+        <v>9</v>
+      </c>
+      <c r="F96" s="24">
+        <v>6</v>
       </c>
       <c r="G96" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H96" s="53">
         <v>1</v>
       </c>
-      <c r="I96" s="56" t="s">
+      <c r="I96" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J96" s="65" t="s">
+      <c r="J96" s="23" t="s">
         <v>82</v>
       </c>
       <c r="K96" s="48">
         <f>E96*F96</f>
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="L96" s="48">
         <f>ROUND(K96/28,1)</f>
-        <v>0.6</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="25.5">
@@ -5262,61 +5292,61 @@
         <v>95</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>202</v>
+        <v>46</v>
       </c>
       <c r="D97" s="55" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E97" s="24">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F97" s="24">
         <v>4</v>
       </c>
-      <c r="G97" s="43" t="s">
+      <c r="G97" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H97" s="53">
-        <v>1</v>
-      </c>
-      <c r="I97" s="55" t="s">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I97" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J97" s="65" t="s">
+      <c r="J97" s="23" t="s">
         <v>82</v>
       </c>
       <c r="K97" s="48">
         <f>E97*F97</f>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="L97" s="48">
         <f>ROUND(K97/28,1)</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="25.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="7"/>
       <c r="B98" s="14">
         <f>B97+1</f>
         <v>96</v>
       </c>
       <c r="C98" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="56" t="s">
-        <v>12</v>
+        <v>124</v>
+      </c>
+      <c r="D98" s="55" t="s">
+        <v>47</v>
       </c>
       <c r="E98" s="52">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F98" s="52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G98" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H98" s="53">
-        <v>0.88900000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="I98" s="56" t="s">
         <v>86</v>
@@ -5326,36 +5356,36 @@
       </c>
       <c r="K98" s="48">
         <f>E98*F98</f>
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="L98" s="48">
         <f>ROUND(K98/28,1)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" ht="25.5">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="7"/>
       <c r="B99" s="14">
         <f>B98+1</f>
         <v>97</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E99" s="35">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F99" s="52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G99" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H99" s="40">
-        <v>0.9</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="I99" s="12" t="s">
         <v>86</v>
@@ -5365,11 +5395,11 @@
       </c>
       <c r="K99" s="47">
         <f>E99*F99</f>
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="L99" s="48">
         <f>ROUND(K99/28,1)</f>
-        <v>0.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="25.5">
@@ -5378,56 +5408,56 @@
         <f>B99+1</f>
         <v>98</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="35">
+      <c r="C100" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E100" s="36">
         <v>4</v>
       </c>
-      <c r="F100" s="52">
-        <v>6</v>
+      <c r="F100" s="24">
+        <v>3</v>
       </c>
       <c r="G100" s="42" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="H100" s="40">
-        <v>0.83299999999999996</v>
+        <v>1</v>
       </c>
       <c r="I100" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J100" s="30" t="s">
+      <c r="J100" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K100" s="47">
         <f>E100*F100</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L100" s="48">
         <f>ROUND(K100/28,1)</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="25.5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="26.25">
       <c r="A101" s="7"/>
       <c r="B101" s="14">
         <f>B100+1</f>
         <v>99</v>
       </c>
-      <c r="C101" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="13" t="s">
+      <c r="C101" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D101" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E101" s="36">
+      <c r="E101" s="35">
         <v>4</v>
       </c>
-      <c r="F101" s="24">
-        <v>3</v>
+      <c r="F101" s="52">
+        <v>4</v>
       </c>
       <c r="G101" s="42" t="s">
         <v>112</v>
@@ -5438,16 +5468,16 @@
       <c r="I101" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J101" s="30" t="s">
+      <c r="J101" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K101" s="47">
         <f>E101*F101</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L101" s="48">
         <f>ROUND(K101/28,1)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="25.5">
@@ -5457,75 +5487,75 @@
         <v>100</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="E102" s="36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F102" s="24">
-        <v>5</v>
-      </c>
-      <c r="G102" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G102" s="43" t="s">
         <v>112</v>
       </c>
       <c r="H102" s="40">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="I102" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J102" s="30" t="s">
+      <c r="J102" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K102" s="47">
         <f>E102*F102</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L102" s="48">
         <f>ROUND(K102/28,1)</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="25.5">
       <c r="A103" s="7"/>
       <c r="B103" s="14">
         <f>B102+1</f>
         <v>101</v>
       </c>
-      <c r="C103" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E103" s="36">
-        <v>5</v>
-      </c>
-      <c r="F103" s="24">
-        <v>4</v>
+      <c r="C103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="35">
+        <v>7</v>
+      </c>
+      <c r="F103" s="52">
+        <v>6</v>
       </c>
       <c r="G103" s="42" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H103" s="40">
-        <v>0.89900000000000002</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="I103" s="12" t="s">
         <v>86</v>
       </c>
       <c r="J103" s="30" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="K103" s="47">
         <f>E103*F103</f>
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="L103" s="48">
         <f>ROUND(K103/28,1)</f>
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="25.5">
@@ -5535,13 +5565,13 @@
         <v>102</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E104" s="35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F104" s="52">
         <v>6</v>
@@ -5550,46 +5580,46 @@
         <v>112</v>
       </c>
       <c r="H104" s="40">
-        <v>0.88900000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="I104" s="12" t="s">
         <v>86</v>
       </c>
       <c r="J104" s="30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K104" s="47">
         <f>E104*F104</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="L104" s="48">
         <f>ROUND(K104/28,1)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="25.5">
       <c r="A105" s="7"/>
       <c r="B105" s="14">
         <f>B104+1</f>
         <v>103</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E105" s="35">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F105" s="52">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G105" s="42" t="s">
         <v>112</v>
       </c>
       <c r="H105" s="40">
-        <v>0.84699999999999998</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="I105" s="12" t="s">
         <v>86</v>
@@ -5599,116 +5629,246 @@
       </c>
       <c r="K105" s="47">
         <f>E105*F105</f>
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="L105" s="48">
         <f>ROUND(K105/28,1)</f>
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="25.5">
       <c r="A106" s="7"/>
       <c r="B106" s="14">
         <f>B105+1</f>
         <v>104</v>
       </c>
-      <c r="C106" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D106" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="E106" s="35">
-        <v>8</v>
-      </c>
-      <c r="F106" s="52">
-        <v>15</v>
-      </c>
-      <c r="G106" s="106" t="s">
+      <c r="C106" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="36">
+        <v>4</v>
+      </c>
+      <c r="F106" s="24">
+        <v>3</v>
+      </c>
+      <c r="G106" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H106" s="103">
-        <v>0.9</v>
-      </c>
-      <c r="I106" s="97" t="s">
+      <c r="H106" s="40">
+        <v>1</v>
+      </c>
+      <c r="I106" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J106" s="25" t="s">
-        <v>180</v>
+      <c r="J106" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="K106" s="47">
         <f>E106*F106</f>
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="L106" s="48">
         <f>ROUND(K106/28,1)</f>
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="25.5">
       <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="H107" s="67"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="15"/>
-      <c r="L107" s="15"/>
+      <c r="B107" s="14">
+        <f>B106+1</f>
+        <v>105</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D107" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="E107" s="24">
+        <v>5</v>
+      </c>
+      <c r="F107" s="24">
+        <v>5</v>
+      </c>
+      <c r="G107" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H107" s="53">
+        <v>0.88</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J107" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K107" s="48">
+        <f>E107*F107</f>
+        <v>25</v>
+      </c>
+      <c r="L107" s="48">
+        <f>ROUND(K107/28,1)</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
-      <c r="H108" s="66"/>
-      <c r="I108" s="5"/>
-      <c r="J108" s="29"/>
-      <c r="K108" s="15"/>
-      <c r="L108" s="15"/>
-    </row>
-    <row r="109" spans="1:12">
+      <c r="B108" s="14">
+        <f>B107+1</f>
+        <v>106</v>
+      </c>
+      <c r="C108" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D108" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="E108" s="24">
+        <v>5</v>
+      </c>
+      <c r="F108" s="24">
+        <v>4</v>
+      </c>
+      <c r="G108" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="H108" s="53">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="I108" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J108" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K108" s="48">
+        <f>E108*F108</f>
+        <v>20</v>
+      </c>
+      <c r="L108" s="48">
+        <f>ROUND(K108/28,1)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="25.5">
       <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="9"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="9"/>
-      <c r="F109" s="9"/>
-      <c r="H109" s="108"/>
-      <c r="I109" s="5"/>
-      <c r="J109" s="29"/>
-      <c r="K109" s="15"/>
-      <c r="L109" s="15"/>
+      <c r="B109" s="14">
+        <f>B108+1</f>
+        <v>107</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" s="52">
+        <v>6</v>
+      </c>
+      <c r="F109" s="52">
+        <v>6</v>
+      </c>
+      <c r="G109" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="H109" s="53">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="I109" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J109" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="K109" s="48">
+        <f>E109*F109</f>
+        <v>36</v>
+      </c>
+      <c r="L109" s="48">
+        <f>ROUND(K109/28,1)</f>
+        <v>1.3</v>
+      </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="9"/>
-      <c r="H110" s="66"/>
-      <c r="I110" s="5"/>
-      <c r="J110" s="29"/>
-      <c r="K110" s="15"/>
-      <c r="L110" s="15"/>
+      <c r="B110" s="14">
+        <f>B109+1</f>
+        <v>108</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D110" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E110" s="52">
+        <v>8</v>
+      </c>
+      <c r="F110" s="52">
+        <v>12</v>
+      </c>
+      <c r="G110" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="H110" s="53">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="I110" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J110" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="K110" s="48">
+        <f>E110*F110</f>
+        <v>96</v>
+      </c>
+      <c r="L110" s="48">
+        <f>ROUND(K110/28,1)</f>
+        <v>3.4</v>
+      </c>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="7"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="9"/>
-      <c r="H111" s="66"/>
-      <c r="I111" s="5"/>
-      <c r="J111" s="29"/>
-      <c r="K111" s="15"/>
-      <c r="L111" s="15"/>
+      <c r="B111" s="14">
+        <f>B110+1</f>
+        <v>109</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D111" s="103" t="s">
+        <v>31</v>
+      </c>
+      <c r="E111" s="52">
+        <v>8</v>
+      </c>
+      <c r="F111" s="52">
+        <v>15</v>
+      </c>
+      <c r="G111" s="112" t="s">
+        <v>112</v>
+      </c>
+      <c r="H111" s="109">
+        <v>0.9</v>
+      </c>
+      <c r="I111" s="111" t="s">
+        <v>86</v>
+      </c>
+      <c r="J111" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="K111" s="48">
+        <f>E111*F111</f>
+        <v>120</v>
+      </c>
+      <c r="L111" s="48">
+        <f>ROUND(K111/28,1)</f>
+        <v>4.3</v>
+      </c>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="7"/>
@@ -5730,7 +5890,7 @@
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
-      <c r="H113" s="109"/>
+      <c r="H113" s="105"/>
       <c r="I113" s="5"/>
       <c r="J113" s="29"/>
       <c r="K113" s="15"/>
@@ -5743,7 +5903,7 @@
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
       <c r="F114" s="9"/>
-      <c r="H114" s="110"/>
+      <c r="H114" s="106"/>
       <c r="I114" s="5"/>
       <c r="J114" s="29"/>
       <c r="K114" s="15"/>
@@ -5782,7 +5942,7 @@
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
-      <c r="H117" s="109"/>
+      <c r="H117" s="105"/>
       <c r="I117" s="5"/>
       <c r="J117" s="29"/>
       <c r="K117" s="15"/>
@@ -5795,7 +5955,7 @@
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
       <c r="F118" s="9"/>
-      <c r="H118" s="111"/>
+      <c r="H118" s="107"/>
       <c r="I118" s="5"/>
       <c r="J118" s="29"/>
       <c r="K118" s="15"/>
@@ -5834,7 +5994,7 @@
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
       <c r="F121" s="9"/>
-      <c r="H121" s="108"/>
+      <c r="H121" s="104"/>
       <c r="I121" s="5"/>
       <c r="J121" s="29"/>
       <c r="K121" s="15"/>
@@ -5847,7 +6007,7 @@
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
-      <c r="H122" s="108"/>
+      <c r="H122" s="104"/>
       <c r="I122" s="5"/>
       <c r="J122" s="29"/>
       <c r="K122" s="15"/>
@@ -6090,7 +6250,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:L106">
-    <sortState ref="B3:L106">
+    <sortState ref="B3:L111">
       <sortCondition ref="D2:D106"/>
     </sortState>
   </autoFilter>
@@ -6210,7 +6370,7 @@
       <c r="G4" s="53">
         <v>1</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="92" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="42">
@@ -6274,7 +6434,7 @@
       <c r="G6" s="40">
         <v>0.91</v>
       </c>
-      <c r="H6" s="93" t="s">
+      <c r="H6" s="92" t="s">
         <v>82</v>
       </c>
       <c r="I6" s="78">
@@ -6307,7 +6467,7 @@
       <c r="G7" s="40">
         <v>0.78</v>
       </c>
-      <c r="H7" s="93" t="s">
+      <c r="H7" s="92" t="s">
         <v>198</v>
       </c>
       <c r="I7" s="78">
@@ -6340,7 +6500,7 @@
       <c r="G8" s="40">
         <v>0.97</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="92" t="s">
         <v>207</v>
       </c>
       <c r="I8" s="42">
@@ -6370,7 +6530,7 @@
       <c r="F9" s="76">
         <v>8</v>
       </c>
-      <c r="G9" s="92">
+      <c r="G9" s="91">
         <v>0.85</v>
       </c>
       <c r="H9" s="77" t="s">
@@ -6437,7 +6597,7 @@
       <c r="G11" s="53">
         <v>0.88</v>
       </c>
-      <c r="H11" s="89" t="s">
+      <c r="H11" s="88" t="s">
         <v>81</v>
       </c>
       <c r="I11" s="78">
@@ -6500,7 +6660,7 @@
       <c r="F13" s="76">
         <v>4</v>
       </c>
-      <c r="G13" s="92">
+      <c r="G13" s="91">
         <v>1</v>
       </c>
       <c r="H13" s="77" t="s">
@@ -6533,10 +6693,10 @@
       <c r="F14" s="52">
         <v>4</v>
       </c>
-      <c r="G14" s="100">
+      <c r="G14" s="99">
         <v>0.81</v>
       </c>
-      <c r="H14" s="89" t="s">
+      <c r="H14" s="88" t="s">
         <v>82</v>
       </c>
       <c r="I14" s="78">
@@ -6569,7 +6729,7 @@
       <c r="G15" s="53">
         <v>1</v>
       </c>
-      <c r="H15" s="89" t="s">
+      <c r="H15" s="88" t="s">
         <v>82</v>
       </c>
       <c r="I15" s="87">
@@ -6602,7 +6762,7 @@
       <c r="G16" s="40">
         <v>0.81</v>
       </c>
-      <c r="H16" s="93" t="s">
+      <c r="H16" s="92" t="s">
         <v>82</v>
       </c>
       <c r="I16" s="78">
@@ -6632,7 +6792,7 @@
       <c r="F17" s="76">
         <v>5</v>
       </c>
-      <c r="G17" s="99">
+      <c r="G17" s="98">
         <v>0.94</v>
       </c>
       <c r="H17" s="77" t="s">
@@ -6666,7 +6826,7 @@
       <c r="G18" s="86">
         <v>0.8</v>
       </c>
-      <c r="H18" s="98" t="s">
+      <c r="H18" s="97" t="s">
         <v>103</v>
       </c>
       <c r="I18" s="87">
@@ -7594,124 +7754,124 @@
         <v>64</v>
       </c>
       <c r="K4" s="48">
-        <f t="shared" ref="K4:K5" si="3">E4*F4</f>
+        <f t="shared" ref="K4" si="3">E4*F4</f>
         <v>36</v>
       </c>
       <c r="L4" s="48">
-        <f t="shared" ref="L4:L5" si="4">ROUND(K4/28,1)</f>
+        <f t="shared" ref="L4" si="4">ROUND(K4/28,1)</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="38.25">
+    <row r="5" spans="1:14" ht="25.5">
       <c r="A5" s="8"/>
       <c r="B5" s="14">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C5" s="70" t="s">
-        <v>215</v>
+      <c r="C5" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="52">
-        <v>6</v>
+        <v>220</v>
+      </c>
+      <c r="E5" s="42">
+        <v>7</v>
       </c>
       <c r="F5" s="52">
-        <v>6</v>
-      </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="12" t="s">
-        <v>122</v>
+        <v>7</v>
+      </c>
+      <c r="G5" s="101"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="39" t="s">
+        <v>86</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="K5" s="48">
-        <f t="shared" si="3"/>
-        <v>36</v>
+        <f t="shared" ref="K5:K7" si="5">E5*F5</f>
+        <v>49</v>
       </c>
       <c r="L5" s="48">
-        <f t="shared" si="4"/>
-        <v>1.3</v>
-      </c>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-    </row>
-    <row r="6" spans="1:14" ht="25.5">
+        <f t="shared" ref="L5:L7" si="6">ROUND(K5/28,1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="M5" s="89"/>
+      <c r="N5" s="89"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="8"/>
       <c r="B6" s="14">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>220</v>
-      </c>
-      <c r="E6" s="42">
-        <v>7</v>
-      </c>
-      <c r="F6" s="52">
-        <v>7</v>
-      </c>
-      <c r="G6" s="102"/>
+      <c r="C6" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="43">
+        <v>4</v>
+      </c>
+      <c r="F6" s="43">
+        <v>9</v>
+      </c>
+      <c r="G6" s="42"/>
       <c r="H6" s="40"/>
-      <c r="I6" s="39" t="s">
-        <v>86</v>
+      <c r="I6" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="K6" s="48">
-        <f t="shared" ref="K6:K7" si="5">E6*F6</f>
-        <v>49</v>
+        <v>64</v>
+      </c>
+      <c r="K6" s="47">
+        <f t="shared" si="5"/>
+        <v>36</v>
       </c>
       <c r="L6" s="48">
-        <f t="shared" ref="L6:L7" si="6">ROUND(K6/28,1)</f>
-        <v>1.8</v>
-      </c>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-    </row>
-    <row r="7" spans="1:14">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+    </row>
+    <row r="7" spans="1:14" ht="25.5">
       <c r="A7" s="8"/>
       <c r="B7" s="14">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="43">
+      <c r="C7" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="35">
+        <v>5</v>
+      </c>
+      <c r="F7" s="42">
         <v>4</v>
       </c>
-      <c r="F7" s="43">
-        <v>9</v>
-      </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="47">
+      <c r="G7" s="52"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="48">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L7" s="48">
         <f t="shared" si="6"/>
-        <v>1.3</v>
-      </c>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
+        <v>0.7</v>
+      </c>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="8"/>
@@ -7719,18 +7879,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="66"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="58"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="29"/>
       <c r="K8" s="49"/>
       <c r="L8" s="49"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="8"/>
@@ -7738,18 +7898,18 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="66"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="29"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="58"/>
       <c r="K9" s="49"/>
       <c r="L9" s="49"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="8"/>
@@ -7757,18 +7917,18 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="H10" s="66"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="58"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="29"/>
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="8"/>
@@ -7776,18 +7936,18 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="35"/>
       <c r="H11" s="66"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="29"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="8"/>
@@ -7801,28 +7961,28 @@
       <c r="F12" s="36"/>
       <c r="G12" s="35"/>
       <c r="H12" s="66"/>
-      <c r="I12" s="6"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="58"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="8"/>
       <c r="B13" s="35"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="H13" s="66"/>
       <c r="I13" s="5"/>
       <c r="J13" s="58"/>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="8"/>
@@ -7855,10 +8015,10 @@
     <row r="16" spans="1:14">
       <c r="A16" s="8"/>
       <c r="B16" s="35"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="35"/>
       <c r="H16" s="66"/>
       <c r="I16" s="5"/>
@@ -7873,9 +8033,9 @@
       <c r="D17" s="6"/>
       <c r="E17" s="36"/>
       <c r="F17" s="36"/>
-      <c r="G17" s="35"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="66"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="58"/>
       <c r="K17" s="49"/>
       <c r="L17" s="49"/>
@@ -7883,13 +8043,13 @@
     <row r="18" spans="1:12">
       <c r="A18" s="8"/>
       <c r="B18" s="35"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="66"/>
-      <c r="I18" s="33"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="58"/>
       <c r="K18" s="49"/>
       <c r="L18" s="49"/>
@@ -7911,15 +8071,15 @@
     <row r="20" spans="1:12">
       <c r="A20" s="8"/>
       <c r="B20" s="35"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="49"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="15"/>
       <c r="L20" s="49"/>
     </row>
     <row r="21" spans="1:12">
@@ -7944,11 +8104,11 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="32"/>
+      <c r="H22" s="57"/>
       <c r="I22" s="33"/>
       <c r="J22" s="29"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="49"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="8"/>
@@ -7958,7 +8118,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="57"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="33"/>
       <c r="J23" s="29"/>
       <c r="K23" s="15"/>
@@ -9074,15 +9234,6 @@
     <row r="104" spans="1:12">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="32"/>
-      <c r="I104" s="33"/>
-      <c r="J104" s="29"/>
-      <c r="K104" s="15"/>
       <c r="L104" s="15"/>
     </row>
     <row r="105" spans="1:12">
@@ -9093,7 +9244,6 @@
     <row r="106" spans="1:12">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
-      <c r="L106" s="15"/>
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="7"/>
@@ -9269,7 +9419,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25">
-      <c r="A1" s="90"/>
+      <c r="A1" s="89"/>
       <c r="B1" s="7"/>
       <c r="C1" s="72" t="s">
         <v>175</v>
@@ -9285,7 +9435,7 @@
       <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="25.5">
-      <c r="A2" s="91"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="79" t="s">
         <v>0</v>
       </c>
@@ -9317,7 +9467,7 @@
       <c r="L2" s="71"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="90"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="74">
         <v>1</v>
       </c>
@@ -9326,14 +9476,14 @@
       <c r="E3" s="52"/>
       <c r="F3" s="42"/>
       <c r="G3" s="40"/>
-      <c r="H3" s="93"/>
+      <c r="H3" s="92"/>
       <c r="I3" s="78"/>
       <c r="J3" s="73"/>
       <c r="K3" s="49"/>
       <c r="L3" s="49"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="90"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="74">
         <f>B3+1</f>
         <v>2</v>
@@ -9343,14 +9493,14 @@
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
       <c r="G4" s="53"/>
-      <c r="H4" s="89"/>
+      <c r="H4" s="88"/>
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="90"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="74">
         <f>B4+1</f>
         <v>3</v>
@@ -9360,14 +9510,14 @@
       <c r="E5" s="42"/>
       <c r="F5" s="52"/>
       <c r="G5" s="53"/>
-      <c r="H5" s="89"/>
+      <c r="H5" s="88"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="90"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="74">
         <f>B5+1</f>
         <v>4</v>
@@ -9377,14 +9527,14 @@
       <c r="E6" s="42"/>
       <c r="F6" s="52"/>
       <c r="G6" s="53"/>
-      <c r="H6" s="89"/>
+      <c r="H6" s="88"/>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
       <c r="K6" s="49"/>
       <c r="L6" s="49"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="90"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="74">
         <f>B6+1</f>
         <v>5</v>
@@ -9402,7 +9552,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="7"/>
-      <c r="B8" s="94"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="15"/>
       <c r="D8" s="29"/>
       <c r="E8" s="35"/>
@@ -9417,7 +9567,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="7"/>
-      <c r="B9" s="94"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="35"/>

</xml_diff>